<commit_message>
Paymethod, paystatus, delivery status error handle
</commit_message>
<xml_diff>
--- a/zzyTest/Order.xlsx
+++ b/zzyTest/Order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LYLJack\Desktop\isemGroupProject\Version2\ISEM_Grop_proj-master\ISEM_Grop_proj\zzyTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B885CF0-1C10-42A0-BA29-424D878115E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAED208-5AF2-483D-AF2B-966BE6274454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,7 +478,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="40" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="94" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>